<commit_message>
modify mutation and fix fitness calculation bug
</commit_message>
<xml_diff>
--- a/data/JSP_dataset.xlsx
+++ b/data/JSP_dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d10b21f834252303/桌面/大三下/專題/GA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="230" documentId="11_C36D2856E769CEEBB9C125721384FA9EE6DCAC47" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89054B35-C1AE-4BB4-A8C5-2B3271DB22C8}"/>
+  <xr:revisionPtr revIDLastSave="289" documentId="11_C36D2856E769CEEBB9C125721384FA9EE6DCAC47" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63B51740-7026-46D6-A40C-BBADB57CF886}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Job Type" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>O1</t>
   </si>
@@ -73,6 +73,42 @@
   </si>
   <si>
     <t>setup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J20</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -141,6 +177,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -406,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -493,10 +533,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -512,10 +552,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -569,10 +609,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -588,10 +628,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -607,10 +647,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -629,7 +669,106 @@
         <v>3</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -640,10 +779,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -704,7 +843,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -721,7 +860,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -738,7 +877,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -755,7 +894,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -772,7 +911,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -789,7 +928,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -806,7 +945,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -823,7 +962,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -840,7 +979,79 @@
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>10</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>